<commit_message>
Added Inserting Dummy Data to DDL
</commit_message>
<xml_diff>
--- a/MOD3_3_Cultural Class Provider_Simulation.xlsx
+++ b/MOD3_3_Cultural Class Provider_Simulation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chris\Desktop\CCINFOM\Cultural-Classes-Provider\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Personal\School\DLSU\Second Year\First Term\CCINFOM S12\Assignments\MP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41FEDC0E-3817-40BB-A031-B45266EDD748}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{443F5F63-A532-4A27-816E-15C196334322}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-8385" yWindow="3300" windowWidth="15375" windowHeight="7875" xr2:uid="{934D5646-0F65-4D73-BFA6-300C2E022D3A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{934D5646-0F65-4D73-BFA6-300C2E022D3A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="102">
   <si>
     <t>system_administrators</t>
   </si>
@@ -249,9 +249,6 @@
     <t>approved_by</t>
   </si>
   <si>
-    <t>cultural classes provider</t>
-  </si>
-  <si>
     <t>cultural_class_providers</t>
   </si>
   <si>
@@ -325,6 +322,24 @@
   </si>
   <si>
     <t>narrative</t>
+  </si>
+  <si>
+    <t>How to Meditate</t>
+  </si>
+  <si>
+    <t>Learn how to meditate through experienced trainers.</t>
+  </si>
+  <si>
+    <t>Time Management</t>
+  </si>
+  <si>
+    <t>Learn how to manage your time with the help of proven time management experts.</t>
+  </si>
+  <si>
+    <t>Jake Trinity</t>
+  </si>
+  <si>
+    <t>Cultural Class Provider</t>
   </si>
 </sst>
 </file>
@@ -693,13 +708,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{782299BD-5059-4B12-A24D-4E2CF9E473BA}">
-  <dimension ref="A1:P75"/>
+  <dimension ref="A1:P77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
-      <selection activeCell="E75" sqref="E75"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="D67" sqref="D67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -1156,7 +1174,7 @@
         <v>303</v>
       </c>
       <c r="C55" t="s">
-        <v>71</v>
+        <v>101</v>
       </c>
       <c r="D55">
         <v>2</v>
@@ -1170,7 +1188,7 @@
     </row>
     <row r="58" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="59" spans="1:16" x14ac:dyDescent="0.25">
@@ -1185,63 +1203,69 @@
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="64" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
+        <v>73</v>
+      </c>
+      <c r="B64" t="s">
         <v>74</v>
-      </c>
-      <c r="B64" t="s">
-        <v>75</v>
       </c>
       <c r="C64" t="s">
         <v>27</v>
       </c>
       <c r="D64" t="s">
+        <v>75</v>
+      </c>
+      <c r="E64" t="s">
         <v>76</v>
       </c>
-      <c r="E64" t="s">
+      <c r="F64" t="s">
         <v>77</v>
       </c>
-      <c r="F64" t="s">
+      <c r="G64" t="s">
         <v>78</v>
       </c>
-      <c r="G64" t="s">
+      <c r="H64" t="s">
         <v>79</v>
       </c>
-      <c r="H64" t="s">
+      <c r="I64" t="s">
         <v>80</v>
       </c>
-      <c r="I64" t="s">
+      <c r="J64" t="s">
         <v>81</v>
       </c>
-      <c r="J64" t="s">
+      <c r="K64" t="s">
         <v>82</v>
       </c>
-      <c r="K64" t="s">
+      <c r="L64" t="s">
         <v>83</v>
       </c>
-      <c r="L64" t="s">
+      <c r="M64" t="s">
         <v>84</v>
       </c>
-      <c r="M64" t="s">
+      <c r="N64" t="s">
         <v>85</v>
       </c>
-      <c r="N64" t="s">
+      <c r="O64" t="s">
         <v>86</v>
       </c>
-      <c r="O64" t="s">
+      <c r="P64" t="s">
         <v>87</v>
-      </c>
-      <c r="P64" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="65" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>12</v>
       </c>
+      <c r="B65" t="s">
+        <v>96</v>
+      </c>
+      <c r="C65" t="s">
+        <v>97</v>
+      </c>
       <c r="D65">
         <v>3</v>
       </c>
@@ -1264,7 +1288,7 @@
         <v>5</v>
       </c>
       <c r="L65" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="M65">
         <v>1</v>
@@ -1273,70 +1297,128 @@
         <v>1</v>
       </c>
       <c r="O65">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P65">
         <v>123</v>
       </c>
     </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A68" s="1" t="s">
+    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>13</v>
+      </c>
+      <c r="B66" t="s">
+        <v>98</v>
+      </c>
+      <c r="C66" t="s">
+        <v>99</v>
+      </c>
+      <c r="D66">
+        <v>4</v>
+      </c>
+      <c r="E66">
+        <v>14.56</v>
+      </c>
+      <c r="F66">
+        <v>120.99</v>
+      </c>
+      <c r="G66" s="2">
+        <v>44256</v>
+      </c>
+      <c r="I66">
+        <v>75</v>
+      </c>
+      <c r="J66">
+        <v>1</v>
+      </c>
+      <c r="K66">
+        <v>5</v>
+      </c>
+      <c r="L66" t="s">
+        <v>100</v>
+      </c>
+      <c r="M66">
+        <v>1</v>
+      </c>
+      <c r="N66">
+        <v>1</v>
+      </c>
+      <c r="O66">
+        <v>0</v>
+      </c>
+      <c r="P66">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>91</v>
+      </c>
+      <c r="B70" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
+      <c r="C70" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>541</v>
+      </c>
+      <c r="B71">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="74" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A74" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="75" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>90</v>
+      </c>
+      <c r="B75" t="s">
+        <v>73</v>
+      </c>
+      <c r="C75" t="s">
+        <v>33</v>
+      </c>
+      <c r="D75" t="s">
+        <v>91</v>
+      </c>
+      <c r="E75" t="s">
         <v>92</v>
       </c>
-      <c r="B69" t="s">
-        <v>95</v>
-      </c>
-      <c r="C69" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A70">
+    </row>
+    <row r="76" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>351</v>
+      </c>
+      <c r="B76">
+        <v>12</v>
+      </c>
+      <c r="C76">
+        <v>301</v>
+      </c>
+      <c r="D76">
         <v>541</v>
       </c>
-      <c r="B70">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A73" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="74" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
-        <v>91</v>
-      </c>
-      <c r="B74" t="s">
-        <v>74</v>
-      </c>
-      <c r="C74" t="s">
-        <v>33</v>
-      </c>
-      <c r="D74" t="s">
-        <v>92</v>
-      </c>
-      <c r="E74" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="75" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A75">
-        <v>351</v>
-      </c>
-      <c r="B75">
-        <v>12</v>
-      </c>
-      <c r="C75">
+    </row>
+    <row r="77" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>352</v>
+      </c>
+      <c r="B77">
+        <v>13</v>
+      </c>
+      <c r="C77">
         <v>301</v>
-      </c>
-      <c r="D75">
-        <v>541</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
corrected differences between excel and sql
</commit_message>
<xml_diff>
--- a/MOD3_3_Cultural Class Provider_Simulation.xlsx
+++ b/MOD3_3_Cultural Class Provider_Simulation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Personal\School\DLSU\Second Year\First Term\CCINFOM S12\Assignments\MP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chris\Desktop\CCINFOM\Cultural-Classes-Provider\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{443F5F63-A532-4A27-816E-15C196334322}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2E2AE7A-1434-463D-AA1B-C76C7BA5D956}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{934D5646-0F65-4D73-BFA6-300C2E022D3A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{934D5646-0F65-4D73-BFA6-300C2E022D3A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="104">
   <si>
     <t>system_administrators</t>
   </si>
@@ -340,6 +340,12 @@
   </si>
   <si>
     <t>Cultural Class Provider</t>
+  </si>
+  <si>
+    <t>It was an amazing class!</t>
+  </si>
+  <si>
+    <t>Payment for Course</t>
   </si>
 </sst>
 </file>
@@ -708,10 +714,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{782299BD-5059-4B12-A24D-4E2CF9E473BA}">
-  <dimension ref="A1:P77"/>
+  <dimension ref="A1:P78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="D67" sqref="D67"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1021,312 +1027,285 @@
       <c r="D34">
         <v>8522</v>
       </c>
+      <c r="E34" t="s">
+        <v>103</v>
+      </c>
       <c r="F34">
         <v>201</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>4322</v>
+      </c>
+      <c r="B35">
+        <v>203</v>
+      </c>
+      <c r="D35">
+        <v>8521</v>
+      </c>
+      <c r="E35" t="s">
+        <v>103</v>
+      </c>
+      <c r="F35">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>48</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B39" t="s">
         <v>49</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C39" t="s">
         <v>50</v>
       </c>
-      <c r="D38" t="s">
+      <c r="D39" t="s">
         <v>51</v>
       </c>
-      <c r="E38" t="s">
+      <c r="E39" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40">
         <v>321</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B40" t="s">
         <v>52</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C40" t="s">
         <v>53</v>
       </c>
-      <c r="D39" t="s">
+      <c r="D40" t="s">
         <v>54</v>
       </c>
-      <c r="E39">
+      <c r="E40">
         <v>201</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>56</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B44" t="s">
         <v>9</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C44" t="s">
         <v>10</v>
       </c>
-      <c r="D43" t="s">
+      <c r="D44" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45">
         <v>1</v>
       </c>
-      <c r="B44" s="2">
+      <c r="B45" s="2">
         <v>44197</v>
       </c>
-      <c r="D44">
+      <c r="D45">
         <v>301</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="1" t="s">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
         <v>33</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B49" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A49">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A50">
         <v>301</v>
-      </c>
-      <c r="B49">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A50">
-        <v>302</v>
       </c>
       <c r="B50">
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A53" s="1" t="s">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>302</v>
+      </c>
+      <c r="B51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
         <v>60</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B55" t="s">
         <v>61</v>
       </c>
-      <c r="C54" t="s">
+      <c r="C55" t="s">
         <v>62</v>
       </c>
-      <c r="D54" t="s">
+      <c r="D55" t="s">
         <v>63</v>
       </c>
-      <c r="E54" t="s">
+      <c r="E55" t="s">
         <v>64</v>
       </c>
-      <c r="F54" t="s">
+      <c r="F55" t="s">
         <v>65</v>
       </c>
-      <c r="G54" t="s">
+      <c r="G55" t="s">
         <v>66</v>
       </c>
-      <c r="H54" t="s">
+      <c r="H55" t="s">
         <v>67</v>
       </c>
-      <c r="I54" t="s">
+      <c r="I55" t="s">
         <v>68</v>
       </c>
-      <c r="J54" t="s">
+      <c r="J55" t="s">
         <v>69</v>
       </c>
-      <c r="K54" t="s">
+      <c r="K55" t="s">
         <v>48</v>
       </c>
-      <c r="L54" t="s">
+      <c r="L55" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A55">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A56">
         <v>123</v>
       </c>
-      <c r="B55">
+      <c r="B56">
         <v>303</v>
       </c>
-      <c r="C55" t="s">
+      <c r="C56" t="s">
         <v>101</v>
       </c>
-      <c r="D55">
+      <c r="D56">
         <v>2</v>
       </c>
-      <c r="K55">
+      <c r="K56">
         <v>321</v>
       </c>
-      <c r="L55">
+      <c r="L56">
         <v>201</v>
       </c>
     </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A58" s="1" t="s">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A60">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A61">
         <v>123</v>
       </c>
     </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A63" s="1" t="s">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
+    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
         <v>73</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B65" t="s">
         <v>74</v>
       </c>
-      <c r="C64" t="s">
+      <c r="C65" t="s">
         <v>27</v>
       </c>
-      <c r="D64" t="s">
+      <c r="D65" t="s">
         <v>75</v>
       </c>
-      <c r="E64" t="s">
+      <c r="E65" t="s">
         <v>76</v>
       </c>
-      <c r="F64" t="s">
+      <c r="F65" t="s">
         <v>77</v>
       </c>
-      <c r="G64" t="s">
+      <c r="G65" t="s">
         <v>78</v>
       </c>
-      <c r="H64" t="s">
+      <c r="H65" t="s">
         <v>79</v>
       </c>
-      <c r="I64" t="s">
+      <c r="I65" t="s">
         <v>80</v>
       </c>
-      <c r="J64" t="s">
+      <c r="J65" t="s">
         <v>81</v>
       </c>
-      <c r="K64" t="s">
+      <c r="K65" t="s">
         <v>82</v>
       </c>
-      <c r="L64" t="s">
+      <c r="L65" t="s">
         <v>83</v>
       </c>
-      <c r="M64" t="s">
+      <c r="M65" t="s">
         <v>84</v>
       </c>
-      <c r="N64" t="s">
+      <c r="N65" t="s">
         <v>85</v>
       </c>
-      <c r="O64" t="s">
+      <c r="O65" t="s">
         <v>86</v>
       </c>
-      <c r="P64" t="s">
+      <c r="P65" t="s">
         <v>87</v>
-      </c>
-    </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A65">
-        <v>12</v>
-      </c>
-      <c r="B65" t="s">
-        <v>96</v>
-      </c>
-      <c r="C65" t="s">
-        <v>97</v>
-      </c>
-      <c r="D65">
-        <v>3</v>
-      </c>
-      <c r="E65" s="3">
-        <v>-28.8</v>
-      </c>
-      <c r="F65" s="3">
-        <v>78.98</v>
-      </c>
-      <c r="G65" s="2">
-        <v>44197</v>
-      </c>
-      <c r="I65">
-        <v>50</v>
-      </c>
-      <c r="J65">
-        <v>1</v>
-      </c>
-      <c r="K65">
-        <v>5</v>
-      </c>
-      <c r="L65" t="s">
-        <v>88</v>
-      </c>
-      <c r="M65">
-        <v>1</v>
-      </c>
-      <c r="N65">
-        <v>1</v>
-      </c>
-      <c r="O65">
-        <v>1</v>
-      </c>
-      <c r="P65">
-        <v>123</v>
       </c>
     </row>
     <row r="66" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A66">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B66" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C66" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D66">
-        <v>4</v>
-      </c>
-      <c r="E66">
-        <v>14.56</v>
-      </c>
-      <c r="F66">
-        <v>120.99</v>
+        <v>3</v>
+      </c>
+      <c r="E66" s="3">
+        <v>-28.8</v>
+      </c>
+      <c r="F66" s="3">
+        <v>78.98</v>
       </c>
       <c r="G66" s="2">
-        <v>44256</v>
+        <v>44197</v>
       </c>
       <c r="I66">
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="J66">
         <v>1</v>
@@ -1335,7 +1314,7 @@
         <v>5</v>
       </c>
       <c r="L66" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="M66">
         <v>1</v>
@@ -1344,80 +1323,130 @@
         <v>1</v>
       </c>
       <c r="O66">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P66">
         <v>123</v>
       </c>
     </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A69" s="1" t="s">
+    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>13</v>
+      </c>
+      <c r="B67" t="s">
+        <v>98</v>
+      </c>
+      <c r="C67" t="s">
+        <v>99</v>
+      </c>
+      <c r="D67">
+        <v>4</v>
+      </c>
+      <c r="E67">
+        <v>14.56</v>
+      </c>
+      <c r="F67">
+        <v>120.99</v>
+      </c>
+      <c r="G67" s="2">
+        <v>44256</v>
+      </c>
+      <c r="I67">
+        <v>75</v>
+      </c>
+      <c r="J67">
+        <v>1</v>
+      </c>
+      <c r="K67">
+        <v>5</v>
+      </c>
+      <c r="L67" t="s">
+        <v>100</v>
+      </c>
+      <c r="M67">
+        <v>1</v>
+      </c>
+      <c r="N67">
+        <v>1</v>
+      </c>
+      <c r="O67">
+        <v>0</v>
+      </c>
+      <c r="P67">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
+    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
         <v>91</v>
       </c>
-      <c r="B70" t="s">
+      <c r="B71" t="s">
         <v>94</v>
       </c>
-      <c r="C70" t="s">
+      <c r="C71" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A71">
+    <row r="72" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A72">
         <v>541</v>
       </c>
-      <c r="B71">
+      <c r="B72">
         <v>5</v>
       </c>
-    </row>
-    <row r="74" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A74" s="1" t="s">
+      <c r="C72" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="75" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A75" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="75" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
+    <row r="76" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
         <v>90</v>
       </c>
-      <c r="B75" t="s">
+      <c r="B76" t="s">
         <v>73</v>
       </c>
-      <c r="C75" t="s">
+      <c r="C76" t="s">
         <v>33</v>
       </c>
-      <c r="D75" t="s">
+      <c r="D76" t="s">
         <v>91</v>
       </c>
-      <c r="E75" t="s">
+      <c r="E76" t="s">
         <v>92</v>
-      </c>
-    </row>
-    <row r="76" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A76">
-        <v>351</v>
-      </c>
-      <c r="B76">
-        <v>12</v>
-      </c>
-      <c r="C76">
-        <v>301</v>
-      </c>
-      <c r="D76">
-        <v>541</v>
       </c>
     </row>
     <row r="77" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A77">
+        <v>351</v>
+      </c>
+      <c r="B77">
+        <v>12</v>
+      </c>
+      <c r="C77">
+        <v>301</v>
+      </c>
+      <c r="D77">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="78" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A78">
         <v>352</v>
       </c>
-      <c r="B77">
+      <c r="B78">
         <v>13</v>
       </c>
-      <c r="C77">
+      <c r="C78">
         <v>301</v>
       </c>
     </row>

</xml_diff>